<commit_message>
Translate values to English for modelling
</commit_message>
<xml_diff>
--- a/notebooks/summary.xlsx
+++ b/notebooks/summary.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,245 +434,300 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>section</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>section_time</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>killed</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>severly_injured</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>lightly_injured</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>injured_pedestrians</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>casualties_ages_0-19</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>casualties_ages_20-64</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>casualties_ages_65_plus</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>total_casualties</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>vehicle_count</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>drivers</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>not_extended_one_lane</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>57</v>
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>not_extended_after_2012</t>
+        </is>
       </c>
       <c r="C2" t="n">
-        <v>131</v>
+        <v>24</v>
       </c>
       <c r="D2" t="n">
-        <v>625</v>
+        <v>69</v>
       </c>
       <c r="E2" t="n">
+        <v>202</v>
+      </c>
+      <c r="F2" t="n">
         <v>2</v>
       </c>
-      <c r="F2" t="n">
-        <v>240</v>
-      </c>
       <c r="G2" t="n">
-        <v>512</v>
+        <v>53</v>
       </c>
       <c r="H2" t="n">
-        <v>51</v>
+        <v>198</v>
       </c>
       <c r="I2" t="n">
-        <v>813</v>
+        <v>35</v>
       </c>
       <c r="J2" t="n">
-        <v>343</v>
+        <v>295</v>
       </c>
       <c r="K2" t="n">
-        <v>343</v>
+        <v>135</v>
+      </c>
+      <c r="L2" t="n">
+        <v>135</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>phase_1_one_lane</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>13</v>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>not_extended_before_2012</t>
+        </is>
       </c>
       <c r="C3" t="n">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D3" t="n">
-        <v>247</v>
+        <v>62</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>423</v>
       </c>
       <c r="F3" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="H3" t="n">
-        <v>5</v>
+        <v>314</v>
       </c>
       <c r="I3" t="n">
-        <v>275</v>
+        <v>16</v>
       </c>
       <c r="J3" t="n">
-        <v>148</v>
+        <v>518</v>
       </c>
       <c r="K3" t="n">
-        <v>148</v>
+        <v>208</v>
+      </c>
+      <c r="L3" t="n">
+        <v>208</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>phase_1_two_lane</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>phase_1_after_2012</t>
+        </is>
+      </c>
       <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
         <v>13</v>
       </c>
-      <c r="D4" t="n">
-        <v>90</v>
-      </c>
       <c r="E4" t="n">
+        <v>91</v>
+      </c>
+      <c r="F4" t="n">
         <v>1</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>27</v>
       </c>
-      <c r="G4" t="n">
-        <v>74</v>
-      </c>
       <c r="H4" t="n">
+        <v>75</v>
+      </c>
+      <c r="I4" t="n">
         <v>2</v>
       </c>
-      <c r="I4" t="n">
-        <v>105</v>
-      </c>
       <c r="J4" t="n">
-        <v>59</v>
+        <v>106</v>
       </c>
       <c r="K4" t="n">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="L4" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>phase_2_one_lane</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>10</v>
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>phase_1_before_2012</t>
+        </is>
       </c>
       <c r="C5" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" t="n">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="E5" t="n">
+        <v>246</v>
+      </c>
+      <c r="F5" t="n">
         <v>1</v>
       </c>
-      <c r="F5" t="n">
-        <v>36</v>
-      </c>
       <c r="G5" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="H5" t="n">
-        <v>2</v>
+        <v>197</v>
       </c>
       <c r="I5" t="n">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="J5" t="n">
-        <v>52</v>
+        <v>274</v>
       </c>
       <c r="K5" t="n">
-        <v>52</v>
+        <v>147</v>
+      </c>
+      <c r="L5" t="n">
+        <v>147</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>phase_2_two_lane</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>5</v>
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>phase_2_after_2012</t>
+        </is>
       </c>
       <c r="C6" t="n">
+        <v>7</v>
+      </c>
+      <c r="D6" t="n">
         <v>0</v>
       </c>
-      <c r="D6" t="n">
-        <v>5</v>
-      </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="F6" t="n">
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H6" t="n">
+        <v>23</v>
+      </c>
+      <c r="I6" t="n">
         <v>2</v>
       </c>
-      <c r="I6" t="n">
-        <v>10</v>
-      </c>
       <c r="J6" t="n">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="K6" t="n">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="L6" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>phase_2_before_2012</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>8</v>
+      </c>
+      <c r="D7" t="n">
+        <v>17</v>
+      </c>
+      <c r="E7" t="n">
+        <v>78</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>27</v>
+      </c>
+      <c r="H7" t="n">
+        <v>74</v>
+      </c>
+      <c r="I7" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" t="n">
+        <v>103</v>
+      </c>
+      <c r="K7" t="n">
+        <v>40</v>
+      </c>
+      <c r="L7" t="n">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>